<commit_message>
22/10/24 pasos 4 a 7 freecodecamp
</commit_message>
<xml_diff>
--- a/documentos/Presupuesto.xlsx
+++ b/documentos/Presupuesto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="PRESUPUESTO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
   <si>
     <t>INGRESOS</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Telefonia</t>
+  </si>
+  <si>
+    <t>Ahorro paseo</t>
   </si>
 </sst>
 </file>
@@ -816,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AO36"/>
+  <dimension ref="A2:AO38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AD38" sqref="AD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelCol="1"/>
@@ -2889,16 +2892,16 @@
         <v>19000</v>
       </c>
       <c r="AC28" s="3">
-        <f t="shared" ref="AC28:AC35" si="17">AA28-AB28</f>
+        <f t="shared" ref="AC28:AC36" si="17">AA28-AB28</f>
         <v>138421.6</v>
       </c>
       <c r="AD28" s="3">
-        <f t="shared" ref="AD28:AD35" si="18">AD$24*B28</f>
+        <f t="shared" ref="AD28:AD36" si="18">AD$24*B28</f>
         <v>50100</v>
       </c>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3">
-        <f t="shared" ref="AF28:AF35" si="19">AD28-AE28</f>
+        <f t="shared" ref="AF28:AF36" si="19">AD28-AE28</f>
         <v>50100</v>
       </c>
       <c r="AG28" s="3">
@@ -2907,7 +2910,7 @@
       </c>
       <c r="AH28" s="3"/>
       <c r="AI28" s="3">
-        <f t="shared" ref="AI28:AI35" si="20">AG28-AH28</f>
+        <f t="shared" ref="AI28:AI36" si="20">AG28-AH28</f>
         <v>0</v>
       </c>
       <c r="AJ28" s="3">
@@ -2916,7 +2919,7 @@
       </c>
       <c r="AK28" s="3"/>
       <c r="AL28" s="3">
-        <f t="shared" ref="AL28:AL35" si="21">AJ28-AK28</f>
+        <f t="shared" ref="AL28:AL36" si="21">AJ28-AK28</f>
         <v>0</v>
       </c>
       <c r="AM28" s="3"/>
@@ -3213,10 +3216,10 @@
     </row>
     <row r="33" spans="1:41">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
       <c r="B33" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -3242,52 +3245,34 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
-      <c r="AA33" s="3">
-        <f>AB24*0.15</f>
-        <v>118066.2</v>
-      </c>
+      <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
-      <c r="AC33" s="3">
-        <f t="shared" si="17"/>
-        <v>118066.2</v>
-      </c>
+      <c r="AC33" s="3"/>
       <c r="AD33" s="3">
         <f t="shared" si="18"/>
-        <v>33400</v>
+        <v>16700</v>
       </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3">
         <f t="shared" si="19"/>
-        <v>33400</v>
-      </c>
-      <c r="AG33" s="3">
-        <f>AH24*0.15</f>
-        <v>0</v>
-      </c>
+        <v>16700</v>
+      </c>
+      <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
-      <c r="AI33" s="3">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="3">
-        <f>AJ24*0.15</f>
-        <v>0</v>
-      </c>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
-      <c r="AL33" s="3">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
+      <c r="AL33" s="3"/>
       <c r="AM33" s="3"/>
       <c r="AN33" s="3"/>
       <c r="AO33" s="3"/>
     </row>
     <row r="34" spans="1:41">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B34" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -3317,21 +3302,19 @@
         <f>AB24*0.15</f>
         <v>118066.2</v>
       </c>
-      <c r="AB34" s="3">
-        <v>200000</v>
-      </c>
+      <c r="AB34" s="3"/>
       <c r="AC34" s="3">
         <f t="shared" si="17"/>
-        <v>-81933.8</v>
+        <v>118066.2</v>
       </c>
       <c r="AD34" s="3">
         <f t="shared" si="18"/>
-        <v>50100</v>
+        <v>33400</v>
       </c>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3">
         <f t="shared" si="19"/>
-        <v>50100</v>
+        <v>33400</v>
       </c>
       <c r="AG34" s="3">
         <f>AH24*0.15</f>
@@ -3357,7 +3340,7 @@
     </row>
     <row r="35" spans="1:41">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B35" s="1">
         <v>0.1</v>
@@ -3387,13 +3370,15 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3">
-        <f>AB24*0.1</f>
-        <v>78710.8</v>
-      </c>
-      <c r="AB35" s="3"/>
+        <f>AB24*0.15</f>
+        <v>118066.2</v>
+      </c>
+      <c r="AB35" s="3">
+        <v>200000</v>
+      </c>
       <c r="AC35" s="3">
         <f t="shared" si="17"/>
-        <v>78710.8</v>
+        <v>-81933.8</v>
       </c>
       <c r="AD35" s="3">
         <f t="shared" si="18"/>
@@ -3405,7 +3390,7 @@
         <v>33400</v>
       </c>
       <c r="AG35" s="3">
-        <f>AH24*0.1</f>
+        <f>AH24*0.15</f>
         <v>0</v>
       </c>
       <c r="AH35" s="3"/>
@@ -3414,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="AJ35" s="3">
-        <f>AJ24*0.1</f>
+        <f>AJ24*0.15</f>
         <v>0</v>
       </c>
       <c r="AK35" s="3"/>
@@ -3428,85 +3413,162 @@
     </row>
     <row r="36" spans="1:41">
       <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3">
+        <f>AB24*0.1</f>
+        <v>78710.8</v>
+      </c>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3">
+        <f t="shared" si="17"/>
+        <v>78710.8</v>
+      </c>
+      <c r="AD36" s="3">
+        <f t="shared" si="18"/>
+        <v>33400</v>
+      </c>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3">
+        <f t="shared" si="19"/>
+        <v>33400</v>
+      </c>
+      <c r="AG36" s="3">
+        <f>AH24*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="3">
+        <f>AJ24*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="3"/>
+      <c r="AO36" s="3"/>
+    </row>
+    <row r="37" spans="1:41">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="1">
-        <f>SUM(B27:B35)</f>
+      <c r="B37" s="1">
+        <f>SUM(B27:B36)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="D36" s="3">
-        <f>SUM(D27:D35)</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="3">
-        <f>SUM(G27:G35)</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="3">
-        <f>SUM(J27:J35)</f>
-        <v>0</v>
-      </c>
-      <c r="M36" s="3">
-        <f>SUM(M27:M35)</f>
-        <v>0</v>
-      </c>
-      <c r="P36" s="3">
-        <f>SUM(P27:P35)</f>
-        <v>0</v>
-      </c>
-      <c r="S36" s="3">
-        <f>SUM(S27:S35)</f>
-        <v>0</v>
-      </c>
-      <c r="V36" s="3">
-        <f>SUM(V27:V35)</f>
-        <v>0</v>
-      </c>
-      <c r="Y36" s="3">
-        <f>SUM(Y27:Y35)</f>
-        <v>0</v>
-      </c>
-      <c r="AA36" s="3">
-        <f>SUM(AA27:AA35)</f>
+      <c r="D37" s="3">
+        <f>SUM(D27:D36)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <f>SUM(G27:G36)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <f>SUM(J27:J36)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <f>SUM(M27:M36)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <f>SUM(P27:P36)</f>
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
+        <f>SUM(S27:S36)</f>
+        <v>0</v>
+      </c>
+      <c r="V37" s="3">
+        <f>SUM(V27:V36)</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="3">
+        <f>SUM(Y27:Y36)</f>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="3">
+        <f>SUM(AA27:AA36)</f>
         <v>905174.2</v>
       </c>
-      <c r="AB36" s="3">
-        <f>SUM(AB27:AB35)</f>
+      <c r="AB37" s="3">
+        <f>SUM(AB27:AB36)</f>
         <v>323000</v>
       </c>
-      <c r="AC36" s="3">
+      <c r="AC37" s="3">
         <f>SUM(AC27:AC27)</f>
         <v>236132.4</v>
       </c>
-      <c r="AD36" s="3">
-        <f>SUM(AD27:AD35)</f>
+      <c r="AD37" s="3">
+        <f>SUM(AD27:AD36)</f>
         <v>334000</v>
       </c>
-      <c r="AE36" s="3">
-        <f>SUM(AE27:AE35)</f>
-        <v>0</v>
-      </c>
-      <c r="AG36" s="3">
-        <f>SUM(AG27:AG35)</f>
-        <v>0</v>
-      </c>
-      <c r="AH36" s="3">
-        <f>SUM(AH27:AH35)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ36" s="3">
-        <f>SUM(AJ27:AJ35)</f>
-        <v>0</v>
-      </c>
-      <c r="AK36" s="3">
-        <f>SUM(AK27:AK35)</f>
-        <v>0</v>
+      <c r="AE37" s="3">
+        <f>SUM(AE27:AE36)</f>
+        <v>0</v>
+      </c>
+      <c r="AG37" s="3">
+        <f>SUM(AG27:AG36)</f>
+        <v>0</v>
+      </c>
+      <c r="AH37" s="3">
+        <f>SUM(AH27:AH36)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="3">
+        <f>SUM(AJ27:AJ36)</f>
+        <v>0</v>
+      </c>
+      <c r="AK37" s="3">
+        <f>SUM(AK27:AK36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41">
+      <c r="AD38" s="3">
+        <f>AD23+AD37</f>
+        <v>1300000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="AC36" formula="1"/>
+    <ignoredError sqref="AC37" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3585,11 +3647,11 @@
         <v>14</v>
       </c>
       <c r="C7" s="5">
-        <f>PRESUPUESTO!AA36</f>
+        <f>PRESUPUESTO!AA37</f>
         <v>905174.2</v>
       </c>
       <c r="D7" s="5">
-        <f>PRESUPUESTO!AB36</f>
+        <f>PRESUPUESTO!AB37</f>
         <v>323000</v>
       </c>
       <c r="E7" s="5">

</xml_diff>